<commit_message>
the final (blow to my mental health) dashboard
</commit_message>
<xml_diff>
--- a/dashboard/sitz_rede_kommentaranteil.xlsx
+++ b/dashboard/sitz_rede_kommentaranteil.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blumj\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blumj\OneDrive\Desktop\final\turbo-broccoli\dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401EA1AE-C125-415C-84FF-38CAD19BB446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44DD28B-0C18-4410-BDAC-6799299DA17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25275" yWindow="495" windowWidth="25005" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25275" yWindow="495" windowWidth="25005" windowHeight="12540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sitz_redeanteil" sheetId="1" r:id="rId1"/>
-    <sheet name="sitz_unterbrochenanteil" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="sitz_unterbrochenanteil" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sitz_redeanteil!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sitz_unterbrochenanteil!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">sitz_unterbrochenanteil!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="11">
   <si>
     <t>WP</t>
   </si>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="A2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,19 +1033,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3E1330-0D80-4D74-BB9E-24F30DC95892}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="6" width="21.21875" customWidth="1"/>
+    <col min="2" max="5" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,13 +1059,10 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1078,15 +1075,11 @@
       <c r="D2">
         <v>33659</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E29" si="0">C2/D2</f>
-        <v>0.97468730502985823</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1099,15 +1092,11 @@
       <c r="D3">
         <v>33659</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>2.5312694970141717E-2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1120,15 +1109,11 @@
       <c r="D4">
         <v>25856</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>0.95853960396039606</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1141,15 +1126,11 @@
       <c r="D5">
         <v>25856</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4.1460396039603963E-2</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1162,15 +1143,11 @@
       <c r="D6">
         <v>20209</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.96511455292196546</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1183,15 +1160,11 @@
       <c r="D7">
         <v>20209</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>3.4885447078034537E-2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1204,15 +1177,11 @@
       <c r="D8">
         <v>33001</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>0.95742553255961937</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1225,15 +1194,11 @@
       <c r="D9">
         <v>33001</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>4.2574467440380598E-2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1246,15 +1211,11 @@
       <c r="D10">
         <v>48494</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0.93279580979090193</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1267,75 +1228,79 @@
       <c r="D11">
         <v>48494</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>6.7204190209098028E-2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>18738</v>
+      </c>
+      <c r="D12">
+        <v>19644</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>906</v>
+      </c>
+      <c r="D13">
+        <v>19644</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>38897</v>
+      </c>
+      <c r="D14">
+        <v>48827</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>9930</v>
+      </c>
+      <c r="D15">
+        <v>48827</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1343,20 +1308,16 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>735</v>
+        <v>728</v>
       </c>
       <c r="D16">
-        <v>771</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0.953307392996109</v>
-      </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>764</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1367,17 +1328,13 @@
         <v>36</v>
       </c>
       <c r="D17">
-        <v>771</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>4.6692607003891051E-2</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>674</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1385,20 +1342,16 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="D18">
-        <v>675</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0.94222222222222218</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>661</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1406,20 +1359,16 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19">
-        <v>675</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>5.7777777777777775E-2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>661</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1427,20 +1376,16 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D20">
-        <v>266</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0.94360902255639101</v>
-      </c>
-      <c r="F20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1448,20 +1393,16 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21">
-        <v>266</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>5.6390977443609019E-2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -1469,20 +1410,16 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22">
-        <v>123</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0.89430894308943087</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -1490,20 +1427,16 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>123</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0.10569105691056911</v>
-      </c>
-      <c r="F23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1511,20 +1444,16 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24">
-        <v>121</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0.88429752066115708</v>
-      </c>
-      <c r="F24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1532,82 +1461,86 @@
         <v>8</v>
       </c>
       <c r="C25">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D25">
-        <v>121</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0.11570247933884298</v>
-      </c>
-      <c r="F25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>6</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>312</v>
+      </c>
+      <c r="D26">
+        <v>327</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>327</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="E28" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>1752</v>
+      </c>
+      <c r="D28">
+        <v>1956</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>7</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="E29" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="C29">
+        <v>204</v>
+      </c>
+      <c r="D29">
+        <v>1956</v>
+      </c>
+      <c r="E29" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{4B3E1330-0D80-4D74-BB9E-24F30DC95892}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F29">
+  <autoFilter ref="A1:E1" xr:uid="{4B3E1330-0D80-4D74-BB9E-24F30DC95892}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>